<commit_message>
Updated scripts and source data loaded.
</commit_message>
<xml_diff>
--- a/Source_data/Amino_acid_and_vitamin_biosynthetic_pw_heatmaps/SAB_MAGs_amino_acids_vitamins_sec_systems_source_data.xlsx
+++ b/Source_data/Amino_acid_and_vitamin_biosynthetic_pw_heatmaps/SAB_MAGs_amino_acids_vitamins_sec_systems_source_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusla\OneDrive\Desktop\Final\Paper\Sponge_metagenomes_2024_Dima_GitHub\Sponge_metagenomes_2024-main\Additional_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03d0ad81bf276083/ThinkPad_working/Sutor/Science/Spongy/Scripts/Sponge_metagenomes_2024/Source_data/Amino_acid_and_vitamin_biosynthetic_pw_heatmaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EF39C8-9FAC-4D1E-8621-79737DC2EA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EF39C8-9FAC-4D1E-8621-79737DC2EA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FD6FAD5E-F6DE-4967-B470-E37824C73071}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="3" activeTab="5" xr2:uid="{FD6FAD5E-F6DE-4967-B470-E37824C73071}"/>
   </bookViews>
   <sheets>
     <sheet name="KEGG_aa_symb_strains_simpl" sheetId="9" r:id="rId1"/>
@@ -579,7 +579,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,7 +655,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,10 +668,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -993,13 +989,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E838DA69-441F-46D9-9F1F-E2978D09EE39}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -1034,7 +1030,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -1069,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -1104,7 +1100,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -1139,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -1174,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -1209,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -1244,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -1279,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -1314,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -1349,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>138</v>
       </c>
@@ -1384,7 +1380,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -1419,7 +1415,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>133</v>
       </c>
@@ -1454,7 +1450,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>134</v>
       </c>
@@ -1489,7 +1485,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -1524,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -1559,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -1594,7 +1590,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -1629,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -1664,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -1699,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>142</v>
       </c>
@@ -1755,16 +1751,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82F7FC4-8056-44F7-9398-8AAA7D68FD5E}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.9140625" customWidth="1"/>
+    <col min="1" max="1" width="23.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -1799,7 +1795,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -1834,7 +1830,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -1869,7 +1865,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1904,7 +1900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -1939,7 +1935,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -1974,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2009,7 +2005,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -2044,7 +2040,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -2079,7 +2075,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2114,7 +2110,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -2149,7 +2145,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>147</v>
       </c>
@@ -2184,7 +2180,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -2219,7 +2215,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -2254,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -2289,7 +2285,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -2324,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>143</v>
       </c>
@@ -2359,7 +2355,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>159</v>
       </c>
@@ -2394,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>160</v>
       </c>
@@ -2454,12 +2450,12 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="1" max="1" width="24.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -2488,7 +2484,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>168</v>
       </c>
@@ -2517,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -2546,7 +2542,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -2575,7 +2571,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -2604,7 +2600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -2633,7 +2629,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -2662,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>167</v>
       </c>
@@ -2691,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -2720,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -2749,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>178</v>
       </c>
@@ -2791,12 +2787,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -2825,7 +2821,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -2854,7 +2850,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -2883,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -2925,9 +2921,9 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>170</v>
       </c>
@@ -2944,7 +2940,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -2964,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2984,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3004,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -3024,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -3044,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -3064,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -3093,23 +3089,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC2AE15-62F9-42C3-BDB4-39A28A9D9DA3}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="20.9140625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="36.08203125" customWidth="1"/>
-    <col min="7" max="7" width="20.9140625" customWidth="1"/>
-    <col min="8" max="9" width="21.9140625" customWidth="1"/>
+    <col min="2" max="2" width="23.47265625" customWidth="1"/>
+    <col min="3" max="3" width="20.89453125" customWidth="1"/>
+    <col min="4" max="4" width="20.3125" customWidth="1"/>
+    <col min="5" max="5" width="22.3125" customWidth="1"/>
+    <col min="6" max="6" width="36.1015625" customWidth="1"/>
+    <col min="7" max="7" width="20.89453125" customWidth="1"/>
+    <col min="8" max="9" width="21.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3138,7 +3134,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3167,7 +3163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3196,7 +3192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3225,7 +3221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3254,7 +3250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3283,7 +3279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3312,7 +3308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3341,7 +3337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3370,7 +3366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -3399,7 +3395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3428,7 +3424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -3457,7 +3453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -3486,7 +3482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3515,7 +3511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -3544,7 +3540,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -3573,7 +3569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -3602,7 +3598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -3631,7 +3627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -3660,7 +3656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -3689,7 +3685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -3718,7 +3714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -3747,7 +3743,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -3776,7 +3772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -3805,7 +3801,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -3834,7 +3830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -3863,7 +3859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -3892,7 +3888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -3921,7 +3917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3950,7 +3946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -3979,7 +3975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -4008,7 +4004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -4037,7 +4033,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -4066,7 +4062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -4095,7 +4091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -4124,7 +4120,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -4153,7 +4149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -4182,7 +4178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -4211,7 +4207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -4240,7 +4236,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -4269,7 +4265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -4298,7 +4294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -4327,7 +4323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -4356,7 +4352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -4385,7 +4381,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -4414,7 +4410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -4443,7 +4439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -4472,7 +4468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -4501,7 +4497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -4530,7 +4526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -4559,7 +4555,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -4588,7 +4584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -4617,7 +4613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -4646,7 +4642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -4675,7 +4671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -4704,7 +4700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>84</v>
       </c>
@@ -4733,7 +4729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -4762,7 +4758,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -4791,7 +4787,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -4820,7 +4816,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -4849,7 +4845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -4878,7 +4874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -4907,7 +4903,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -4936,7 +4932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>99</v>
       </c>
@@ -4965,7 +4961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -4994,7 +4990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -5023,7 +5019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -5052,7 +5048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -5081,7 +5077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -5110,7 +5106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>105</v>
       </c>
@@ -5139,7 +5135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>106</v>
       </c>

</xml_diff>